<commit_message>
5 experiments without landmark
</commit_message>
<xml_diff>
--- a/Vision/img/experiment_data.xlsx
+++ b/Vision/img/experiment_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JD\Desktop\HPcode\Vision\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2448C41-6708-4C1C-8840-C11F0D4668A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B599D6-480D-45F7-ADA7-7A2E1DDB832C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -398,35 +398,35 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
         <v>-50</v>
-      </c>
-      <c r="B2">
-        <v>90</v>
-      </c>
-      <c r="C2">
-        <v>-40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>50</v>
+        <v>-45</v>
       </c>
       <c r="B3">
-        <v>-90</v>
+        <v>90</v>
       </c>
       <c r="C3">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>-50</v>
+        <v>90</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>-90</v>
       </c>
       <c r="C4">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -442,33 +442,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B6">
-        <v>-40</v>
+        <v>-90</v>
       </c>
       <c r="C6">
         <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>-90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>